<commit_message>
validate button adn download works
</commit_message>
<xml_diff>
--- a/files/reporte-convenios.xlsx
+++ b/files/reporte-convenios.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -76,6 +76,9 @@
     <t>convenio2</t>
   </si>
   <si>
+    <t>12/02/2021</t>
+  </si>
+  <si>
     <t>sector</t>
   </si>
   <si>
@@ -85,6 +88,9 @@
     <t>unam</t>
   </si>
   <si>
+    <t>judith</t>
+  </si>
+  <si>
     <t>periodo4</t>
   </si>
   <si>
@@ -110,6 +116,51 @@
   </si>
   <si>
     <t>convenio43</t>
+  </si>
+  <si>
+    <t>120912lpñl</t>
+  </si>
+  <si>
+    <t>354135</t>
+  </si>
+  <si>
+    <t>poderes de los pobres</t>
+  </si>
+  <si>
+    <t>industrial</t>
+  </si>
+  <si>
+    <t>no se</t>
+  </si>
+  <si>
+    <t>peridos</t>
+  </si>
+  <si>
+    <t>454654</t>
+  </si>
+  <si>
+    <t>algo ninteres</t>
+  </si>
+  <si>
+    <t>sector2</t>
+  </si>
+  <si>
+    <t>Poder</t>
+  </si>
+  <si>
+    <t>EUA</t>
+  </si>
+  <si>
+    <t>periodo555</t>
+  </si>
+  <si>
+    <t>541354</t>
+  </si>
+  <si>
+    <t>poderesss</t>
+  </si>
+  <si>
+    <t>sector23</t>
   </si>
 </sst>
 </file>
@@ -148,10 +199,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +541,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="18" width="10" customWidth="1"/>
@@ -569,26 +619,26 @@
       <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2">
-        <v>44689.29166666667</v>
+      <c r="F2" t="s">
+        <v>21</v>
       </c>
       <c r="G2">
         <v>1321354</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2">
         <v>354354</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -604,6 +654,9 @@
       </c>
       <c r="Q2">
         <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -614,34 +667,34 @@
         <v>12356</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="2">
-        <v>44693.29166666667</v>
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
       </c>
       <c r="G3">
         <v>6516</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I3">
         <v>354135</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M3">
         <v>2</v>
@@ -657,6 +710,9 @@
       </c>
       <c r="Q3">
         <v>0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -667,34 +723,34 @@
         <v>123562</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2">
-        <v>44693.29166666667</v>
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
       </c>
       <c r="G4">
         <v>65162</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I4">
         <v>3541352</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M4">
         <v>2</v>
@@ -709,7 +765,178 @@
         <v>2</v>
       </c>
       <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>354135</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <v>1354</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5">
+        <v>354354</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
         <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>65465</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>543645</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6">
+        <v>654654</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>65432</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <v>54354</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7">
+        <v>321354</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>